<commit_message>
- Update my diary-Yilin Wang.xlsx
</commit_message>
<xml_diff>
--- a/diaries/diary-Yilin Wang.xlsx
+++ b/diaries/diary-Yilin Wang.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlwan\Documents\Study\reverse engineering\SWE265P\diaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlwan\Documents\Study\reverse_engineering\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681102A4-CAD3-4431-B4E4-CDE469E16A7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E219A3-DFA2-491B-BD77-56F0B2677D80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -112,6 +112,21 @@
   </si>
   <si>
     <t>Not bad, not good.</t>
+  </si>
+  <si>
+    <t>Xiaolue Peng, Lindsay Garcia</t>
+  </si>
+  <si>
+    <t>Learn how to read source code</t>
+  </si>
+  <si>
+    <t>Find a beacon to start reading code.Know about the influence of familiarity. Know about how to What's real life of software engineer</t>
+  </si>
+  <si>
+    <t>When looking at new code project, it's normal to feel overwhelming and confused. Starting to find the beacon or using the find to search key words, reading could be easier.</t>
+  </si>
+  <si>
+    <t>Awesome.</t>
   </si>
 </sst>
 </file>
@@ -279,14 +294,14 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="19" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -608,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -618,24 +633,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
@@ -727,10 +742,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A10" s="11">
+      <c r="A10" s="10">
         <v>43839</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="11">
         <v>0.90277777777777779</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -749,27 +764,27 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>8</v>
+    <row r="11" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="10">
+        <v>43846</v>
+      </c>
+      <c r="B11" s="11">
+        <v>0.90972222222222221</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
- Update my diary-Yilin Wang.xlsx (#77)
</commit_message>
<xml_diff>
--- a/diaries/diary-Yilin Wang.xlsx
+++ b/diaries/diary-Yilin Wang.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlwan\Documents\Study\reverse engineering\SWE265P\diaries\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlwan\Documents\Study\reverse_engineering\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681102A4-CAD3-4431-B4E4-CDE469E16A7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E219A3-DFA2-491B-BD77-56F0B2677D80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -112,6 +112,21 @@
   </si>
   <si>
     <t>Not bad, not good.</t>
+  </si>
+  <si>
+    <t>Xiaolue Peng, Lindsay Garcia</t>
+  </si>
+  <si>
+    <t>Learn how to read source code</t>
+  </si>
+  <si>
+    <t>Find a beacon to start reading code.Know about the influence of familiarity. Know about how to What's real life of software engineer</t>
+  </si>
+  <si>
+    <t>When looking at new code project, it's normal to feel overwhelming and confused. Starting to find the beacon or using the find to search key words, reading could be easier.</t>
+  </si>
+  <si>
+    <t>Awesome.</t>
   </si>
 </sst>
 </file>
@@ -279,14 +294,14 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="19" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -608,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -618,24 +633,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
@@ -727,10 +742,10 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="31" x14ac:dyDescent="0.35">
-      <c r="A10" s="11">
+      <c r="A10" s="10">
         <v>43839</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="11">
         <v>0.90277777777777779</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -749,27 +764,27 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>8</v>
+    <row r="11" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="10">
+        <v>43846</v>
+      </c>
+      <c r="B11" s="11">
+        <v>0.90972222222222221</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
- Update diary-Yilin Wang.xlsx
</commit_message>
<xml_diff>
--- a/diaries/diary-Yilin Wang.xlsx
+++ b/diaries/diary-Yilin Wang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlwan\Documents\Study\reverse_engineering\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6B1C3D-647D-4CB0-A5EF-085DFA3EB441}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699AF40A-E3DE-436A-9B3D-BA8804DC3838}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -66,12 +66,6 @@
     <t>Achievements</t>
   </si>
   <si>
-    <t>&lt;how did you feel during the activity?&gt;</t>
-  </si>
-  <si>
-    <t>Etc.</t>
-  </si>
-  <si>
     <t>Yilin Wang</t>
   </si>
   <si>
@@ -121,6 +115,30 @@
   </si>
   <si>
     <t>Get a sense of how to read code efficiently.Installed the SimpleUMLce and build the graph by it.Use metrics.</t>
+  </si>
+  <si>
+    <t>Know more about Git</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have more sense what Git is and What's the good manner to use Git </t>
+  </si>
+  <si>
+    <t>Keep master branch clean.Always update items in different branches.</t>
+  </si>
+  <si>
+    <t>Good.</t>
+  </si>
+  <si>
+    <t>Start this week's assignment</t>
+  </si>
+  <si>
+    <t>Determine two key features of our projects</t>
+  </si>
+  <si>
+    <t>UML is really helpful for understanding sourcce code and the logic behind the code.</t>
+  </si>
+  <si>
+    <t>Tired but great.</t>
   </si>
 </sst>
 </file>
@@ -259,7 +277,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -296,6 +314,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -615,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
-  <dimension ref="A1:G125"/>
+  <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -660,7 +681,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -673,7 +694,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -686,7 +707,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -743,19 +764,19 @@
         <v>0.90277777777777779</v>
       </c>
       <c r="C10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="F10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="G10" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
@@ -766,19 +787,19 @@
         <v>0.90972222222222221</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="F11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="G11" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
@@ -789,40 +810,66 @@
         <v>0.89583333333333337</v>
       </c>
       <c r="C12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="7" t="s">
+      <c r="G12" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="10">
+        <v>43856</v>
+      </c>
+      <c r="B13" s="11">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+      <c r="A14" s="10">
+        <v>43858</v>
+      </c>
+      <c r="B14" s="13">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8"/>
+      <c r="F14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="15" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="7"/>
@@ -843,19 +890,19 @@
       <c r="G16" s="8"/>
     </row>
     <row r="17" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="6"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="8"/>
@@ -864,7 +911,7 @@
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
+      <c r="D19" s="6"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="8"/>
@@ -891,7 +938,7 @@
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
+      <c r="D22" s="8"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="8"/>
@@ -1822,6 +1869,15 @@
       <c r="E125" s="7"/>
       <c r="F125" s="7"/>
       <c r="G125" s="8"/>
+    </row>
+    <row r="126" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A126" s="7"/>
+      <c r="B126" s="7"/>
+      <c r="C126" s="7"/>
+      <c r="D126" s="7"/>
+      <c r="E126" s="7"/>
+      <c r="F126" s="7"/>
+      <c r="G126" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
- Update diaries/diary-Yilin Wang.xlsx
</commit_message>
<xml_diff>
--- a/diaries/diary-Yilin Wang.xlsx
+++ b/diaries/diary-Yilin Wang.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlwan\Documents\Study\reverse_engineering\W2020\diaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699AF40A-E3DE-436A-9B3D-BA8804DC3838}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3569E7BC-FDFD-47AD-8443-769FA4F245E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>SWE 265P Diary</t>
   </si>
@@ -139,6 +139,18 @@
   </si>
   <si>
     <t>Tired but great.</t>
+  </si>
+  <si>
+    <t>Lindsay</t>
+  </si>
+  <si>
+    <t>Get ideas about homeworks and learn from my collegues.</t>
+  </si>
+  <si>
+    <t>Always looks for important feature and find testcases</t>
+  </si>
+  <si>
+    <t>Focus on essence. UML notations. Try to understand the story behind the code.</t>
   </si>
 </sst>
 </file>
@@ -312,11 +324,11 @@
     <xf numFmtId="19" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="18" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="18" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -638,36 +650,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="34.6328125" customWidth="1"/>
+    <col min="1" max="7" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-    </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+    </row>
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -676,7 +688,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -689,7 +701,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -702,7 +714,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -715,7 +727,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -724,7 +736,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -733,7 +745,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -756,7 +768,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <v>43839</v>
       </c>
@@ -779,7 +791,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="78" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <v>43846</v>
       </c>
@@ -802,7 +814,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>43853</v>
       </c>
@@ -825,7 +837,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <v>43856</v>
       </c>
@@ -848,11 +860,11 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <v>43858</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="12">
         <v>0.63888888888888895</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -871,16 +883,30 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="10">
+        <v>43860</v>
+      </c>
+      <c r="B15" s="12">
+        <v>0.75</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -889,7 +915,7 @@
       <c r="F16" s="7"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -898,7 +924,7 @@
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
@@ -907,7 +933,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -916,7 +942,7 @@
       <c r="F19" s="7"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -925,7 +951,7 @@
       <c r="F20" s="7"/>
       <c r="G20" s="8"/>
     </row>
-    <row r="21" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -934,7 +960,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -943,7 +969,7 @@
       <c r="F22" s="7"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -952,7 +978,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -961,7 +987,7 @@
       <c r="F24" s="7"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -970,7 +996,7 @@
       <c r="F25" s="7"/>
       <c r="G25" s="8"/>
     </row>
-    <row r="26" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -979,7 +1005,7 @@
       <c r="F26" s="7"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -988,7 +1014,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -997,7 +1023,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="7"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -1006,7 +1032,7 @@
       <c r="F29" s="7"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="7"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -1015,7 +1041,7 @@
       <c r="F30" s="7"/>
       <c r="G30" s="8"/>
     </row>
-    <row r="31" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1024,7 +1050,7 @@
       <c r="F31" s="7"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -1033,7 +1059,7 @@
       <c r="F32" s="7"/>
       <c r="G32" s="8"/>
     </row>
-    <row r="33" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -1042,7 +1068,7 @@
       <c r="F33" s="7"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -1051,7 +1077,7 @@
       <c r="F34" s="7"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="7"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -1060,7 +1086,7 @@
       <c r="F35" s="7"/>
       <c r="G35" s="8"/>
     </row>
-    <row r="36" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1069,7 +1095,7 @@
       <c r="F36" s="7"/>
       <c r="G36" s="8"/>
     </row>
-    <row r="37" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -1078,7 +1104,7 @@
       <c r="F37" s="7"/>
       <c r="G37" s="8"/>
     </row>
-    <row r="38" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -1087,7 +1113,7 @@
       <c r="F38" s="7"/>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -1096,7 +1122,7 @@
       <c r="F39" s="7"/>
       <c r="G39" s="8"/>
     </row>
-    <row r="40" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -1105,7 +1131,7 @@
       <c r="F40" s="7"/>
       <c r="G40" s="8"/>
     </row>
-    <row r="41" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -1114,7 +1140,7 @@
       <c r="F41" s="7"/>
       <c r="G41" s="8"/>
     </row>
-    <row r="42" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="7"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -1123,7 +1149,7 @@
       <c r="F42" s="7"/>
       <c r="G42" s="8"/>
     </row>
-    <row r="43" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="7"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -1132,7 +1158,7 @@
       <c r="F43" s="7"/>
       <c r="G43" s="8"/>
     </row>
-    <row r="44" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="7"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -1141,7 +1167,7 @@
       <c r="F44" s="7"/>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="7"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -1150,7 +1176,7 @@
       <c r="F45" s="7"/>
       <c r="G45" s="8"/>
     </row>
-    <row r="46" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -1159,7 +1185,7 @@
       <c r="F46" s="7"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="7"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -1168,7 +1194,7 @@
       <c r="F47" s="7"/>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="7"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -1177,7 +1203,7 @@
       <c r="F48" s="7"/>
       <c r="G48" s="8"/>
     </row>
-    <row r="49" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="7"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -1186,7 +1212,7 @@
       <c r="F49" s="7"/>
       <c r="G49" s="8"/>
     </row>
-    <row r="50" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -1195,7 +1221,7 @@
       <c r="F50" s="7"/>
       <c r="G50" s="8"/>
     </row>
-    <row r="51" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="7"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -1204,7 +1230,7 @@
       <c r="F51" s="7"/>
       <c r="G51" s="8"/>
     </row>
-    <row r="52" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="7"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -1213,7 +1239,7 @@
       <c r="F52" s="7"/>
       <c r="G52" s="8"/>
     </row>
-    <row r="53" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="7"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -1222,7 +1248,7 @@
       <c r="F53" s="7"/>
       <c r="G53" s="8"/>
     </row>
-    <row r="54" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -1231,7 +1257,7 @@
       <c r="F54" s="7"/>
       <c r="G54" s="8"/>
     </row>
-    <row r="55" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="7"/>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -1240,7 +1266,7 @@
       <c r="F55" s="7"/>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -1249,7 +1275,7 @@
       <c r="F56" s="7"/>
       <c r="G56" s="8"/>
     </row>
-    <row r="57" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
@@ -1258,7 +1284,7 @@
       <c r="F57" s="7"/>
       <c r="G57" s="8"/>
     </row>
-    <row r="58" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="7"/>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
@@ -1267,7 +1293,7 @@
       <c r="F58" s="7"/>
       <c r="G58" s="8"/>
     </row>
-    <row r="59" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="7"/>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
@@ -1276,7 +1302,7 @@
       <c r="F59" s="7"/>
       <c r="G59" s="8"/>
     </row>
-    <row r="60" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="7"/>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -1285,7 +1311,7 @@
       <c r="F60" s="7"/>
       <c r="G60" s="8"/>
     </row>
-    <row r="61" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="7"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -1294,7 +1320,7 @@
       <c r="F61" s="7"/>
       <c r="G61" s="8"/>
     </row>
-    <row r="62" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="7"/>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -1303,7 +1329,7 @@
       <c r="F62" s="7"/>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="7"/>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -1312,7 +1338,7 @@
       <c r="F63" s="7"/>
       <c r="G63" s="8"/>
     </row>
-    <row r="64" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="7"/>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -1321,7 +1347,7 @@
       <c r="F64" s="7"/>
       <c r="G64" s="8"/>
     </row>
-    <row r="65" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="7"/>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -1330,7 +1356,7 @@
       <c r="F65" s="7"/>
       <c r="G65" s="8"/>
     </row>
-    <row r="66" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -1339,7 +1365,7 @@
       <c r="F66" s="7"/>
       <c r="G66" s="8"/>
     </row>
-    <row r="67" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="7"/>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
@@ -1348,7 +1374,7 @@
       <c r="F67" s="7"/>
       <c r="G67" s="8"/>
     </row>
-    <row r="68" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="7"/>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
@@ -1357,7 +1383,7 @@
       <c r="F68" s="7"/>
       <c r="G68" s="8"/>
     </row>
-    <row r="69" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -1366,7 +1392,7 @@
       <c r="F69" s="7"/>
       <c r="G69" s="8"/>
     </row>
-    <row r="70" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="7"/>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -1375,7 +1401,7 @@
       <c r="F70" s="7"/>
       <c r="G70" s="8"/>
     </row>
-    <row r="71" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="7"/>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
@@ -1384,7 +1410,7 @@
       <c r="F71" s="7"/>
       <c r="G71" s="8"/>
     </row>
-    <row r="72" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="7"/>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
@@ -1393,7 +1419,7 @@
       <c r="F72" s="7"/>
       <c r="G72" s="8"/>
     </row>
-    <row r="73" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="7"/>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
@@ -1402,7 +1428,7 @@
       <c r="F73" s="7"/>
       <c r="G73" s="8"/>
     </row>
-    <row r="74" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="7"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -1411,7 +1437,7 @@
       <c r="F74" s="7"/>
       <c r="G74" s="8"/>
     </row>
-    <row r="75" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="7"/>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -1420,7 +1446,7 @@
       <c r="F75" s="7"/>
       <c r="G75" s="8"/>
     </row>
-    <row r="76" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -1429,7 +1455,7 @@
       <c r="F76" s="7"/>
       <c r="G76" s="8"/>
     </row>
-    <row r="77" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="7"/>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
@@ -1438,7 +1464,7 @@
       <c r="F77" s="7"/>
       <c r="G77" s="8"/>
     </row>
-    <row r="78" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="7"/>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
@@ -1447,7 +1473,7 @@
       <c r="F78" s="7"/>
       <c r="G78" s="8"/>
     </row>
-    <row r="79" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
@@ -1456,7 +1482,7 @@
       <c r="F79" s="7"/>
       <c r="G79" s="8"/>
     </row>
-    <row r="80" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="7"/>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -1465,7 +1491,7 @@
       <c r="F80" s="7"/>
       <c r="G80" s="8"/>
     </row>
-    <row r="81" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="7"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
@@ -1474,7 +1500,7 @@
       <c r="F81" s="7"/>
       <c r="G81" s="8"/>
     </row>
-    <row r="82" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
@@ -1483,7 +1509,7 @@
       <c r="F82" s="7"/>
       <c r="G82" s="8"/>
     </row>
-    <row r="83" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="7"/>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
@@ -1492,7 +1518,7 @@
       <c r="F83" s="7"/>
       <c r="G83" s="8"/>
     </row>
-    <row r="84" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="7"/>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
@@ -1501,7 +1527,7 @@
       <c r="F84" s="7"/>
       <c r="G84" s="8"/>
     </row>
-    <row r="85" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="7"/>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
@@ -1510,7 +1536,7 @@
       <c r="F85" s="7"/>
       <c r="G85" s="8"/>
     </row>
-    <row r="86" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="7"/>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -1519,7 +1545,7 @@
       <c r="F86" s="7"/>
       <c r="G86" s="8"/>
     </row>
-    <row r="87" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
@@ -1528,7 +1554,7 @@
       <c r="F87" s="7"/>
       <c r="G87" s="8"/>
     </row>
-    <row r="88" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="7"/>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
@@ -1537,7 +1563,7 @@
       <c r="F88" s="7"/>
       <c r="G88" s="8"/>
     </row>
-    <row r="89" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="7"/>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
@@ -1546,7 +1572,7 @@
       <c r="F89" s="7"/>
       <c r="G89" s="8"/>
     </row>
-    <row r="90" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -1555,7 +1581,7 @@
       <c r="F90" s="7"/>
       <c r="G90" s="8"/>
     </row>
-    <row r="91" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="7"/>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
@@ -1564,7 +1590,7 @@
       <c r="F91" s="7"/>
       <c r="G91" s="8"/>
     </row>
-    <row r="92" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="7"/>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -1573,7 +1599,7 @@
       <c r="F92" s="7"/>
       <c r="G92" s="8"/>
     </row>
-    <row r="93" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="7"/>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -1582,7 +1608,7 @@
       <c r="F93" s="7"/>
       <c r="G93" s="8"/>
     </row>
-    <row r="94" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="7"/>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -1591,7 +1617,7 @@
       <c r="F94" s="7"/>
       <c r="G94" s="8"/>
     </row>
-    <row r="95" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="7"/>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -1600,7 +1626,7 @@
       <c r="F95" s="7"/>
       <c r="G95" s="8"/>
     </row>
-    <row r="96" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="7"/>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -1609,7 +1635,7 @@
       <c r="F96" s="7"/>
       <c r="G96" s="8"/>
     </row>
-    <row r="97" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" s="7"/>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
@@ -1618,7 +1644,7 @@
       <c r="F97" s="7"/>
       <c r="G97" s="8"/>
     </row>
-    <row r="98" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
@@ -1627,7 +1653,7 @@
       <c r="F98" s="7"/>
       <c r="G98" s="8"/>
     </row>
-    <row r="99" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="7"/>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
@@ -1636,7 +1662,7 @@
       <c r="F99" s="7"/>
       <c r="G99" s="8"/>
     </row>
-    <row r="100" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="7"/>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -1645,7 +1671,7 @@
       <c r="F100" s="7"/>
       <c r="G100" s="8"/>
     </row>
-    <row r="101" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A101" s="7"/>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -1654,7 +1680,7 @@
       <c r="F101" s="7"/>
       <c r="G101" s="8"/>
     </row>
-    <row r="102" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A102" s="7"/>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -1663,7 +1689,7 @@
       <c r="F102" s="7"/>
       <c r="G102" s="8"/>
     </row>
-    <row r="103" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A103" s="7"/>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -1672,7 +1698,7 @@
       <c r="F103" s="7"/>
       <c r="G103" s="8"/>
     </row>
-    <row r="104" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="7"/>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -1681,7 +1707,7 @@
       <c r="F104" s="7"/>
       <c r="G104" s="8"/>
     </row>
-    <row r="105" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A105" s="7"/>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -1690,7 +1716,7 @@
       <c r="F105" s="7"/>
       <c r="G105" s="8"/>
     </row>
-    <row r="106" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="7"/>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -1699,7 +1725,7 @@
       <c r="F106" s="7"/>
       <c r="G106" s="8"/>
     </row>
-    <row r="107" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -1708,7 +1734,7 @@
       <c r="F107" s="7"/>
       <c r="G107" s="8"/>
     </row>
-    <row r="108" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A108" s="7"/>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -1717,7 +1743,7 @@
       <c r="F108" s="7"/>
       <c r="G108" s="8"/>
     </row>
-    <row r="109" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" s="7"/>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
@@ -1726,7 +1752,7 @@
       <c r="F109" s="7"/>
       <c r="G109" s="8"/>
     </row>
-    <row r="110" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
@@ -1735,7 +1761,7 @@
       <c r="F110" s="7"/>
       <c r="G110" s="8"/>
     </row>
-    <row r="111" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A111" s="7"/>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
@@ -1744,7 +1770,7 @@
       <c r="F111" s="7"/>
       <c r="G111" s="8"/>
     </row>
-    <row r="112" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A112" s="7"/>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
@@ -1753,7 +1779,7 @@
       <c r="F112" s="7"/>
       <c r="G112" s="8"/>
     </row>
-    <row r="113" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" s="7"/>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
@@ -1762,7 +1788,7 @@
       <c r="F113" s="7"/>
       <c r="G113" s="8"/>
     </row>
-    <row r="114" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A114" s="7"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
@@ -1771,7 +1797,7 @@
       <c r="F114" s="7"/>
       <c r="G114" s="8"/>
     </row>
-    <row r="115" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A115" s="7"/>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
@@ -1780,7 +1806,7 @@
       <c r="F115" s="7"/>
       <c r="G115" s="8"/>
     </row>
-    <row r="116" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
@@ -1789,7 +1815,7 @@
       <c r="F116" s="7"/>
       <c r="G116" s="8"/>
     </row>
-    <row r="117" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
@@ -1798,7 +1824,7 @@
       <c r="F117" s="7"/>
       <c r="G117" s="8"/>
     </row>
-    <row r="118" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
@@ -1807,7 +1833,7 @@
       <c r="F118" s="7"/>
       <c r="G118" s="8"/>
     </row>
-    <row r="119" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
@@ -1816,7 +1842,7 @@
       <c r="F119" s="7"/>
       <c r="G119" s="8"/>
     </row>
-    <row r="120" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A120" s="7"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
@@ -1825,7 +1851,7 @@
       <c r="F120" s="7"/>
       <c r="G120" s="8"/>
     </row>
-    <row r="121" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121" s="7"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
@@ -1834,7 +1860,7 @@
       <c r="F121" s="7"/>
       <c r="G121" s="8"/>
     </row>
-    <row r="122" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
@@ -1843,7 +1869,7 @@
       <c r="F122" s="7"/>
       <c r="G122" s="8"/>
     </row>
-    <row r="123" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
@@ -1852,7 +1878,7 @@
       <c r="F123" s="7"/>
       <c r="G123" s="8"/>
     </row>
-    <row r="124" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" s="7"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
@@ -1861,7 +1887,7 @@
       <c r="F124" s="7"/>
       <c r="G124" s="8"/>
     </row>
-    <row r="125" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A125" s="7"/>
       <c r="B125" s="7"/>
       <c r="C125" s="7"/>
@@ -1870,7 +1896,7 @@
       <c r="F125" s="7"/>
       <c r="G125" s="8"/>
     </row>
-    <row r="126" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A126" s="7"/>
       <c r="B126" s="7"/>
       <c r="C126" s="7"/>

</xml_diff>